<commit_message>
1.Separeted the app for public, user and admin logic; 2.Started to build admin logic
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -669,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +771,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>3</v>
@@ -783,7 +783,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>5</v>
@@ -1022,7 +1022,9 @@
       <c r="B32" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="5">
+        <v>5</v>
+      </c>
       <c r="D32" s="5" t="s">
         <v>5</v>
       </c>
@@ -1212,7 +1214,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
Implemented admin delete user and admin edit user functionalities
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Galabov</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -669,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,7 +1045,9 @@
       <c r="B34" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="7"/>
+      <c r="C34" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="D34" s="7" t="s">
         <v>28</v>
       </c>
@@ -1052,7 +1057,9 @@
       <c r="B35" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="7"/>
+      <c r="C35" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="D35" s="7" t="s">
         <v>28</v>
       </c>
@@ -1062,7 +1069,9 @@
       <c r="B36" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="7"/>
+      <c r="C36" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="D36" s="7" t="s">
         <v>28</v>
       </c>
@@ -1072,7 +1081,9 @@
       <c r="B37" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="D37" s="7" t="s">
         <v>28</v>
       </c>
@@ -1082,7 +1093,9 @@
       <c r="B38" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="D38" s="7" t="s">
         <v>28</v>
       </c>
@@ -1092,7 +1105,9 @@
       <c r="B39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="D39" s="7" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
List towns, fixed some bugs
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -672,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,7 +777,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>3</v>
@@ -1117,7 +1120,9 @@
       <c r="B40" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="7"/>
+      <c r="C40" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="D40" s="7" t="s">
         <v>28</v>
       </c>
@@ -1127,7 +1132,9 @@
       <c r="B41" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="7"/>
+      <c r="C41" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="D41" s="7" t="s">
         <v>28</v>
       </c>
@@ -1137,7 +1144,9 @@
       <c r="B42" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="7"/>
+      <c r="C42" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="D42" s="7" t="s">
         <v>28</v>
       </c>
@@ -1147,7 +1156,9 @@
       <c r="B43" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="7"/>
+      <c r="C43" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D43" s="7" t="s">
         <v>28</v>
       </c>
@@ -1157,7 +1168,9 @@
       <c r="B44" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="7"/>
+      <c r="C44" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D44" s="7" t="s">
         <v>28</v>
       </c>
@@ -1187,7 +1200,9 @@
       <c r="B47" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="7"/>
+      <c r="C47" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D47" s="7" t="s">
         <v>28</v>
       </c>
@@ -1197,7 +1212,9 @@
       <c r="B48" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="7"/>
+      <c r="C48" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="D48" s="7" t="s">
         <v>28</v>
       </c>
@@ -1229,7 +1246,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>